<commit_message>
update db after long non-consistency
</commit_message>
<xml_diff>
--- a/public/db/Base.xlsx
+++ b/public/db/Base.xlsx
@@ -539,19 +539,19 @@
     <t>КПУ-2Н, ниппельный, нормально открытый</t>
   </si>
   <si>
-    <t>59d08e254fd856a3999347fc9decaebd</t>
+    <t>1753277370d4ac6947b80252811a8927</t>
   </si>
   <si>
     <t>КПУ-2Н, ниппельный, нормально закрытый</t>
   </si>
   <si>
-    <t>5026141d680ec7389cc9ff1a436253a0</t>
+    <t>5b97739120375bd47c3ae50d3950e58d</t>
   </si>
   <si>
     <t>КПУ-2Н-ВД, канальный, нормально открытый</t>
   </si>
   <si>
-    <t>0b5a927f5ca0871e8381865e10b43177</t>
+    <t>dbf81601cf5c17223bea2860580b3418</t>
   </si>
   <si>
     <t>https://www.veza.ru/produktsiya/klapany-i-setevye-elementy/protivopozharnye-klapany/pryamougolnye-protivopozharnye-klapany/kpu-2n-pryamougolnye</t>
@@ -565,7 +565,7 @@
     <t>КПУ-2Н-ВД, канальный, нормально закрытый</t>
   </si>
   <si>
-    <t>95552d5b1b1c47a3531781219083398c</t>
+    <t>280c6fce5b59c62e1dfd48172a2b4057</t>
   </si>
   <si>
     <t>1xЭП: 100x100...1000x1500;
@@ -1200,10 +1200,10 @@
     <t>(150x150)x(100x100)...(2000x1400)x(1400x1400)</t>
   </si>
   <si>
-    <t>Воздуховод (Размер, Скорость, Расход, Потеря давления)</t>
-  </si>
-  <si>
-    <t>7f5d79c664692bc497ba2e990b66e08d</t>
+    <t>Воздуховод (4 параметра)</t>
+  </si>
+  <si>
+    <t>b3fecc43137e617af4aa576ec4217dee</t>
   </si>
   <si>
     <t>Выноска автоматически определяет форму воздуховода и делает выбор между обозначением круглого и прямоугольного воздуховодов</t>
@@ -3840,8 +3840,8 @@
   <sheetPr/>
   <dimension ref="B4:V113"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="J92" workbookViewId="0">
-      <selection activeCell="P109" sqref="P109"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -8468,11 +8468,8 @@
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F108;F5:F86;F97:F107;F109:F113">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F86;F97:F113">
       <formula1>Категория_сайта</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K108;K5:K83;K96:K107;K109:K113">
-      <formula1>Тип_графики</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G78">
       <formula1>Категория_техническая</formula1>
@@ -8482,6 +8479,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J52;J109:J113">
       <formula1>Производитель</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5:K83;K96:K113">
+      <formula1>Тип_графики</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q5:V93;Q97:V113">
       <formula1>"ДА"</formula1>
@@ -9444,7 +9444,7 @@
       </c>
       <c r="E15" t="str">
         <f>IF(Компоненты!E15&lt;&gt;"",Компоненты!E15,"")</f>
-        <v>59d08e254fd856a3999347fc9decaebd</v>
+        <v>1753277370d4ac6947b80252811a8927</v>
       </c>
       <c r="F15" t="str">
         <f>IF(Компоненты!F15&lt;&gt;"",Компоненты!F15,"")</f>
@@ -9528,7 +9528,7 @@
       </c>
       <c r="E16" t="str">
         <f>IF(Компоненты!E16&lt;&gt;"",Компоненты!E16,"")</f>
-        <v>5026141d680ec7389cc9ff1a436253a0</v>
+        <v>5b97739120375bd47c3ae50d3950e58d</v>
       </c>
       <c r="F16" t="str">
         <f>IF(Компоненты!F16&lt;&gt;"",Компоненты!F16,"")</f>
@@ -9612,7 +9612,7 @@
       </c>
       <c r="E17" t="str">
         <f>IF(Компоненты!E17&lt;&gt;"",Компоненты!E17,"")</f>
-        <v>0b5a927f5ca0871e8381865e10b43177</v>
+        <v>dbf81601cf5c17223bea2860580b3418</v>
       </c>
       <c r="F17" t="str">
         <f>IF(Компоненты!F17&lt;&gt;"",Компоненты!F17,"")</f>
@@ -9696,7 +9696,7 @@
       </c>
       <c r="E18" t="str">
         <f>IF(Компоненты!E18&lt;&gt;"",Компоненты!E18,"")</f>
-        <v>95552d5b1b1c47a3531781219083398c</v>
+        <v>280c6fce5b59c62e1dfd48172a2b4057</v>
       </c>
       <c r="F18" t="str">
         <f>IF(Компоненты!F18&lt;&gt;"",Компоненты!F18,"")</f>
@@ -15115,7 +15115,7 @@
       </c>
       <c r="C84" t="str">
         <f>IF(Компоненты!C84&lt;&gt;"",Компоненты!C84,"")</f>
-        <v>Воздуховод (Размер, Скорость, Расход, Потеря давления)</v>
+        <v>Воздуховод (4 параметра)</v>
       </c>
       <c r="D84">
         <f>IF(Компоненты!D84&lt;&gt;"",Компоненты!D84,"")</f>
@@ -15123,7 +15123,7 @@
       </c>
       <c r="E84" t="str">
         <f>IF(Компоненты!E84&lt;&gt;"",Компоненты!E84,"")</f>
-        <v>7f5d79c664692bc497ba2e990b66e08d</v>
+        <v>b3fecc43137e617af4aa576ec4217dee</v>
       </c>
       <c r="F84" t="str">
         <f>IF(Компоненты!F84&lt;&gt;"",Компоненты!F84,"")</f>

</xml_diff>